<commit_message>
minor tweaks to the scripts
</commit_message>
<xml_diff>
--- a/competitive programming.xlsx
+++ b/competitive programming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngminpark/Documents/Programming/competitiveprogramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED364D1-A35B-3A45-8F5E-9AB2DA218A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CDFAE-2E75-844D-B60F-8FA10F60B0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17120" xr2:uid="{066B7B58-6DE3-F343-B97B-AF0CF6D8B99C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{066B7B58-6DE3-F343-B97B-AF0CF6D8B99C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
   <si>
     <t>Problem</t>
   </si>
@@ -218,6 +218,54 @@
   </si>
   <si>
     <t>Instead of considering the maximum dp ending with a certain index, consider the reverse: maximum dp starting with a certain index</t>
+  </si>
+  <si>
+    <t>Bitaro</t>
+  </si>
+  <si>
+    <t>Sqrt decomp</t>
+  </si>
+  <si>
+    <t>Tried to label nodes (light, heavy). Realized the graph is acylic</t>
+  </si>
+  <si>
+    <t>Don't always try to sqrt decomp the nodes, but consider other things that could be sqrt decomp</t>
+  </si>
+  <si>
+    <t>Divide queries into heavy queries and light queries. Use mergesort to ensure O(N + M)</t>
+  </si>
+  <si>
+    <t>USACO 2008 Gold</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>O(N^2) DP or O(NlogN)  slope trick type beat</t>
+  </si>
+  <si>
+    <t>koosaga blog post</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Considering the DP_i, j = (x &lt;= j) min(DP_i-1, x), and seeing the unimodality of the DP_i --&gt; Maintaining the optimal points where the slope changes (only in the negatives)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APIO 2019 </t>
+  </si>
+  <si>
+    <t>Bridges</t>
+  </si>
+  <si>
+    <t>editorial</t>
+  </si>
+  <si>
+    <t>Square root decomposition on queries</t>
+  </si>
+  <si>
+    <t>Square root decomp on queries - O(sqrt(Q)) block</t>
+  </si>
+  <si>
+    <t>Always go for the easy solution in contests (in this case the O(N^2) solution is very straightforward)</t>
   </si>
 </sst>
 </file>
@@ -596,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F88911-E763-A445-BEF2-9A1A8259CEC8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,7 +911,7 @@
       <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>57</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -874,6 +922,75 @@
       </c>
       <c r="H11" s="1" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added debug.h, removed range namespace from template
</commit_message>
<xml_diff>
--- a/competitive programming.xlsx
+++ b/competitive programming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngminpark/Documents/Programming/competitiveprogramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CDFAE-2E75-844D-B60F-8FA10F60B0C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597813B0-0A18-6446-8242-C11FA5DC830A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{066B7B58-6DE3-F343-B97B-AF0CF6D8B99C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{066B7B58-6DE3-F343-B97B-AF0CF6D8B99C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="120">
   <si>
     <t>Problem</t>
   </si>
@@ -266,6 +266,135 @@
   </si>
   <si>
     <t>Always go for the easy solution in contests (in this case the O(N^2) solution is very straightforward)</t>
+  </si>
+  <si>
+    <t>USACO 2018 Platinum</t>
+  </si>
+  <si>
+    <t>Open P3 - Disruption</t>
+  </si>
+  <si>
+    <t>Small-to-large</t>
+  </si>
+  <si>
+    <t>Editorial :(</t>
+  </si>
+  <si>
+    <t>Misread the question big time. Read slowly? Read some books?</t>
+  </si>
+  <si>
+    <t>Maintaining a set for each vertex and when merging the sets, erase the element if it has already appeared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atcoder </t>
+  </si>
+  <si>
+    <t>ARC59C</t>
+  </si>
+  <si>
+    <t>DP, Adhoc</t>
+  </si>
+  <si>
+    <t>Read the word DP in the editorial</t>
+  </si>
+  <si>
+    <t>Misread again lmaooo. Slow down I guess</t>
+  </si>
+  <si>
+    <t>Simple DP over the number of children and candies (2D). Expressing DP_{i, j} as a j variable expression helps a lot</t>
+  </si>
+  <si>
+    <t>Baltic OI 2019</t>
+  </si>
+  <si>
+    <t>Valley</t>
+  </si>
+  <si>
+    <t>DP, binary jumping</t>
+  </si>
+  <si>
+    <t>Read editorial</t>
+  </si>
+  <si>
+    <t>The idea to root the tree on the escape vertex. Shift perspectives? Wishful thinking</t>
+  </si>
+  <si>
+    <t>Simple tree DP using binary jumping</t>
+  </si>
+  <si>
+    <t>2016 Code Festival C</t>
+  </si>
+  <si>
+    <t>DP, Adhoc?</t>
+  </si>
+  <si>
+    <t>Read editorial lololol</t>
+  </si>
+  <si>
+    <t>Analyzing when W = 2, generalizing the result using the fact that the relative order can always be satisfied</t>
+  </si>
+  <si>
+    <t>For each column i do a 2D dp on the number of rows removed. Also, the optimization from O(H^3) to O(H^2) per column is needed. To do this, note that we can precalculate the value added when we do the operation for pairs of the form (x, 0), (0, y) and the relationship between (i + 1, j + 1) and (i, j) is easy to spot</t>
+  </si>
+  <si>
+    <t>POI 2011</t>
+  </si>
+  <si>
+    <t>Tree Rotation</t>
+  </si>
+  <si>
+    <t>Small-to-large, Ordered set</t>
+  </si>
+  <si>
+    <t>Realizing two subtrees are independent</t>
+  </si>
+  <si>
+    <t>Do not be afraid of using ordered set if needed</t>
+  </si>
+  <si>
+    <t>Ordered set small to large merging --&gt; O(nlog^2n)</t>
+  </si>
+  <si>
+    <t>IX Samara Regional Intercollegiate Programming contest 2016</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Exchange argument DP, DAG</t>
+  </si>
+  <si>
+    <t>Noticing that the graph has to be a DAG --&gt; considered N = 2 cases and the dp states</t>
+  </si>
+  <si>
+    <t>If the problem is about an optimal ordering of vertices in a DAG, consider the reverse graph (lexicographically minimum/DP problems)</t>
+  </si>
+  <si>
+    <t>Sort by dp_i and do a topsort bfs using a priority_queue</t>
+  </si>
+  <si>
+    <t>Codeforces</t>
+  </si>
+  <si>
+    <t>455E</t>
+  </si>
+  <si>
+    <t>CHT DP Come on</t>
+  </si>
+  <si>
+    <t>Snake Escaping</t>
+  </si>
+  <si>
+    <t>SOS DP, bitmask enumeration</t>
+  </si>
+  <si>
+    <t>Noticing that 2^{L/3} per query is sufficient</t>
+  </si>
+  <si>
+    <t>Submask enumeration only takes 2^{set bits} lmaoooo</t>
+  </si>
+  <si>
+    <t>Supermask, submask sum. For each query use the character that appears the least to ensure 2 ^ {L / 3}, also PIE helps</t>
   </si>
 </sst>
 </file>
@@ -644,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F88911-E763-A445-BEF2-9A1A8259CEC8}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -993,6 +1122,184 @@
         <v>75</v>
       </c>
     </row>
+    <row r="15" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2900</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added a proper Suffix Array template & organized the OI folder
</commit_message>
<xml_diff>
--- a/competitive programming.xlsx
+++ b/competitive programming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/youngminpark/Documents/Programming/competitiveprogramming/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B338C-B289-384F-9D58-86D98951E52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{772EAE4D-334B-D346-A156-0AE86D53BC30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17020" xr2:uid="{066B7B58-6DE3-F343-B97B-AF0CF6D8B99C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="296">
   <si>
     <t>Problem</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Counting the contribution of each subarray. Consider the limits. Think about the combinatorics</t>
   </si>
   <si>
-    <t>Lucas Theroem + contribution</t>
-  </si>
-  <si>
     <t>1673F</t>
   </si>
   <si>
@@ -298,9 +295,6 @@
     <t>Read the word DP in the editorial</t>
   </si>
   <si>
-    <t>Misread again lmaooo. Slow down I guess</t>
-  </si>
-  <si>
     <t>Simple DP over the number of children and candies (2D). Expressing DP_{i, j} as a j variable expression helps a lot</t>
   </si>
   <si>
@@ -505,9 +499,6 @@
     <t>Queries with two types of query: insertion, query, and query values are cumulative. --&gt; Can be solved using CDQ DnC which allows it to use methods that are used to solve the simple version of insertion first then query. Also, this form of FFT is called "online FFT".</t>
   </si>
   <si>
-    <t>DP transition is just convoultion</t>
-  </si>
-  <si>
     <t>1083E</t>
   </si>
   <si>
@@ -598,6 +589,9 @@
     <t>1656F</t>
   </si>
   <si>
+    <t>Upsolving</t>
+  </si>
+  <si>
     <t>Adhoc, MST, Greedy</t>
   </si>
   <si>
@@ -755,6 +749,180 @@
   </si>
   <si>
     <t>Palindrome --&gt; Palindromic tree</t>
+  </si>
+  <si>
+    <t>1644F</t>
+  </si>
+  <si>
+    <t>Combinatorics, SQRT</t>
+  </si>
+  <si>
+    <t>Got everything except for the Stirling's number recurrence</t>
+  </si>
+  <si>
+    <t>Cool trick: The use of the stirling's numbers</t>
+  </si>
+  <si>
+    <t>DP transition is just convolution</t>
+  </si>
+  <si>
+    <t>Misread again. Slow down I guess</t>
+  </si>
+  <si>
+    <t>Lucas Theorem + contribution</t>
+  </si>
+  <si>
+    <t>ARC122D</t>
+  </si>
+  <si>
+    <t>Game theory, xor, trie</t>
+  </si>
+  <si>
+    <t>I had the right idea of iterating over the highest bit</t>
+  </si>
+  <si>
+    <t>Cool trick: For some bitmask problems, consider splitting the set into two groups, one with the ith bit on, and the other with the ith bit off, and then we merge the set in the end. D&amp;C recursion. Also, new variable idea: L for level. I should've thought about the process of going down if even, calculate if odd</t>
+  </si>
+  <si>
+    <t>Iterate over the ith bit position. If there is an odd number of elements with the ith bit on, then we calculate the minimum xor between the sets. Otherwise, we move down another level twice and combine the answer.</t>
+  </si>
+  <si>
+    <t>DMOJ</t>
+  </si>
+  <si>
+    <t>Knapsack4</t>
+  </si>
+  <si>
+    <t>Randomization, knapsack</t>
+  </si>
+  <si>
+    <t>Straightforward DP results in O((N+M)\sigma W)--&gt; randomization</t>
+  </si>
+  <si>
+    <t>Cool trick: For certain knapsack problems, we could reduce the number of states considered via shuffling the array and assuming that the optimal subset is included within a certain range</t>
+  </si>
+  <si>
+    <t>dp_{i, j} where i is the number of people considered and j is the difference of sum1 and sum2</t>
+  </si>
+  <si>
+    <t>CodeChef</t>
+  </si>
+  <si>
+    <t>SHAIKHGN</t>
+  </si>
+  <si>
+    <t>Matrix, bitset optimization</t>
+  </si>
+  <si>
+    <t>Normal matrix multiplication O(MN^2logK)--&gt;bitset</t>
+  </si>
+  <si>
+    <t>Cool trick: When multiplying a product of matrices with a vector, change it to a repeated multiplications between a vector and a matrix</t>
+  </si>
+  <si>
+    <t>Simple matrix multiplication using bitsets</t>
+  </si>
+  <si>
+    <t>APIO 2013</t>
+  </si>
+  <si>
+    <t>Toll</t>
+  </si>
+  <si>
+    <t>MST</t>
+  </si>
+  <si>
+    <t>Considered what edges could be on the  MST in the end</t>
+  </si>
+  <si>
+    <t>Advice: Try to reduce the problem as much as possible from the original form. Even if the problem seems unsolvable, with enough observations, it becomes solvable</t>
+  </si>
+  <si>
+    <t>The edges that are not on the initial MST are first discarded as they would never be on the MST. Now, the number of edges that limit the costs of Mr.Greedy's roads are bounded by k, so we could compress the tree into k subcomponents and do a simple O(k^2) DP per bitmask gives the time complexity, O(k^2*2^k + m\alpha(n))</t>
+  </si>
+  <si>
+    <t>BOI 2010</t>
+  </si>
+  <si>
+    <t>Candies</t>
+  </si>
+  <si>
+    <t>Knapsack, bitset</t>
+  </si>
+  <si>
+    <t>Knapsack--&gt;bitset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advice: Write down concrete equations/observations. </t>
+  </si>
+  <si>
+    <t>Solvied</t>
+  </si>
+  <si>
+    <t>First, we can find the optimal value that should be removed via simple bitmask and then to find Q, we do a similar process, but we use both a_i and -a_i.</t>
+  </si>
+  <si>
+    <t>AGC17D</t>
+  </si>
+  <si>
+    <t>Sprague-Grundy, green Hackenbush</t>
+  </si>
+  <si>
+    <t>Game--&gt;hackenbush--&gt;SG</t>
+  </si>
+  <si>
+    <t>Cool trick: When solving a game theory related problems, consider if it can be reduced into a few subgames where we can apply SG theorem</t>
+  </si>
+  <si>
+    <t>Calculate the SG(u) for each subtree by noticing that adding one edge to the root makes the SG(u) increase by 1.</t>
+  </si>
+  <si>
+    <t>COCI 2015</t>
+  </si>
+  <si>
+    <t>UZASTOPNI</t>
+  </si>
+  <si>
+    <t>Bitset, tree dp</t>
+  </si>
+  <si>
+    <t>Knapsack can take a lot of form, and even if it isn't directly knapsack, consider it</t>
+  </si>
+  <si>
+    <t>For each node, we calculate the boolean arrays lo and hi which are calculated in a knapsack fashion using the values from the child nodes. Think of the ranges as blocks for a knapsack</t>
+  </si>
+  <si>
+    <t>1716F</t>
+  </si>
+  <si>
+    <t>Combinatorics, stirling number</t>
+  </si>
+  <si>
+    <t>Sum of F^k? --&gt; Number of ordered k-tuples--&gt; Partitioning? --&gt; Stirling</t>
+  </si>
+  <si>
+    <t>Cool trick: Always consider swapping the summands if the problem seems to be unsolvable. It makes life easier</t>
+  </si>
+  <si>
+    <t>Sum of F^k is essentially the occurrences of all possible k-tuples of indices that have an odd-numbered ball, which can be calculated by iterating over the number of distinct indices that show up in the k-tuples, and we can think of the number of k-tuples with that j indices as an ordered integer partition of 1..k, so S(k, j)*j!. This solves the first subproblem. Now, we have to consider the number of ways of selecting j indices from 1..n, and filling j balls with odd integers, and the rest (m-j) with even integers. The formula we get is similar to binomial theorem, and we can differentiate a few times to derive a nice clean O(k) solution</t>
+  </si>
+  <si>
+    <t>APIO 2012</t>
+  </si>
+  <si>
+    <t>Dispatching</t>
+  </si>
+  <si>
+    <t>Small-to-large, tree</t>
+  </si>
+  <si>
+    <t>Tree DP?--&gt;Storing the minimum costs of ninjas per subtree--&gt;small-to-large</t>
+  </si>
+  <si>
+    <t>Cool trick: Use priority_queues over multisets if possible as red-black trees suck (the c++ implementation at least)</t>
+  </si>
+  <si>
+    <t>We maintain the minimum costs of ninjas that we can afford for each subtree. Then, we can do a small-to-large merging, and whenever the value exceeds the budget, we remove the most expensive ninja. This doesn't degenerate into a O(n^2) solution since whenever we insert an element, we would have to remove at most one ninja to keep the budget below the limit.</t>
   </si>
 </sst>
 </file>
@@ -1142,10 +1310,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86F88911-E763-A445-BEF2-9A1A8259CEC8}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="143" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,10 +1321,10 @@
     <col min="1" max="1" width="11.33203125" style="1" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="33.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1290,7 +1458,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1310,7 +1478,7 @@
         <v>33</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>34</v>
+        <v>244</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -1318,401 +1486,401 @@
         <v>25</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="D9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="1" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G16" s="1" t="s">
+    </row>
+    <row r="17" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="D17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1">
         <v>2900</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="G22" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F22" s="1" t="s">
+    </row>
+    <row r="23" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="D23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="85" x14ac:dyDescent="0.2">
@@ -1720,27 +1888,27 @@
         <v>8</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="G25" s="1" t="s">
+    </row>
+    <row r="26" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="B26" s="1">
         <v>13514</v>
@@ -1749,21 +1917,21 @@
         <v>10</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B27" s="1">
         <v>13545</v>
@@ -1772,39 +1940,39 @@
         <v>10</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="G27" s="1" t="s">
+    </row>
+    <row r="28" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="136" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+      <c r="D28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="G28" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="H28" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="136" x14ac:dyDescent="0.2">
@@ -1812,22 +1980,22 @@
         <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G29" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>156</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -1835,22 +2003,22 @@
         <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="H30" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="187" x14ac:dyDescent="0.2">
@@ -1858,25 +2026,25 @@
         <v>25</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C31" s="1">
         <v>2500</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="68" x14ac:dyDescent="0.2">
@@ -1884,25 +2052,25 @@
         <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C32" s="1">
         <v>2900</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H32" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="187" x14ac:dyDescent="0.2">
@@ -1910,25 +2078,25 @@
         <v>8</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C33" s="1">
         <v>2397</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -1936,22 +2104,22 @@
         <v>25</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="170" x14ac:dyDescent="0.2">
@@ -1959,22 +2127,22 @@
         <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -1982,45 +2150,45 @@
         <v>25</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D36" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -2028,22 +2196,22 @@
         <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -2051,22 +2219,22 @@
         <v>8</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="H39" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="170" x14ac:dyDescent="0.2">
@@ -2074,22 +2242,22 @@
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="136" x14ac:dyDescent="0.2">
@@ -2097,30 +2265,30 @@
         <v>8</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C42" s="1">
         <v>2700</v>
@@ -2129,16 +2297,16 @@
         <v>10</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -2146,7 +2314,7 @@
         <v>25</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C43" s="1">
         <v>2200</v>
@@ -2155,16 +2323,16 @@
         <v>10</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="H43" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -2172,71 +2340,301 @@
         <v>25</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C44" s="1">
         <v>2700</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G44" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="187" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="D45" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="D45" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="G45" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="F46" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="F46" s="1" t="s">
+    </row>
+    <row r="47" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C47" s="1">
+        <v>2900</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="G46" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>238</v>
+      <c r="F47" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="153" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="170" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>